<commit_message>
fix para exceles con rows vacias
</commit_message>
<xml_diff>
--- a/IPP.xlsx
+++ b/IPP.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_DEV\super-herramientas-redles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\emore\Desktop\super-herramientas-redles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA06B72-B18F-443D-A332-A3E08C8F746F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="585" windowWidth="15495" windowHeight="10185" xr2:uid="{0A6B3FB1-2A93-4383-B760-741B0BB64FBC}"/>
+    <workbookView xWindow="480" yWindow="585" windowWidth="15495" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Explicacion" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>apellidos</t>
   </si>
@@ -116,13 +115,19 @@
   </si>
   <si>
     <t>31279875</t>
+  </si>
+  <si>
+    <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>22/05/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +146,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -202,6 +215,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,14 +530,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFDB6A9B-AE7B-4C94-BC93-F1B60347D67E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -591,8 +606,8 @@
       <c r="H2" s="2">
         <v>15161504</v>
       </c>
-      <c r="I2" s="2">
-        <v>44329</v>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="J2" s="2">
         <v>32737943</v>
@@ -623,8 +638,8 @@
       <c r="H3" s="2">
         <v>15511857</v>
       </c>
-      <c r="I3" s="2">
-        <v>44205</v>
+      <c r="I3" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="J3" s="2">
         <v>32737943</v>
@@ -637,14 +652,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85297140-4713-435D-825E-515455E27BCC}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A1:B11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1"/>
@@ -763,8 +778,8 @@
       <c r="H16" s="2">
         <v>15161504</v>
       </c>
-      <c r="I16" s="2">
-        <v>44329</v>
+      <c r="I16" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="J16" s="2">
         <v>32737943</v>
@@ -795,12 +810,15 @@
       <c r="H17" s="2">
         <v>15511857</v>
       </c>
-      <c r="I17" s="2">
-        <v>44205</v>
+      <c r="I17" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="J17" s="2">
         <v>32737943</v>
       </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>